<commit_message>
connectors, core407z & kinetis files
</commit_message>
<xml_diff>
--- a/Core407_pinout_compare.xlsx
+++ b/Core407_pinout_compare.xlsx
@@ -266,7 +266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -360,11 +360,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -393,6 +408,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -696,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AM22"/>
+  <dimension ref="A2:AM31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1190,7 @@
         <v>24</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="5" t="s">
         <v>51</v>
       </c>
       <c r="I7" s="6" t="s">
@@ -1187,7 +1206,7 @@
         <v>224</v>
       </c>
       <c r="M7" s="7"/>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="O7" s="5"/>
@@ -1254,7 +1273,7 @@
         <v>25</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I8" s="6" t="s">
@@ -1321,7 +1340,7 @@
       <c r="A9" s="16">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="5"/>
@@ -1335,7 +1354,7 @@
         <v>26</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="6" t="s">
@@ -1406,7 +1425,7 @@
       <c r="A10" s="16">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1495,7 +1514,7 @@
       <c r="A11" s="16">
         <v>7</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -2187,7 +2206,7 @@
         <v>211</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="8" t="s">
         <v>30</v>
       </c>
       <c r="I19" s="5"/>
@@ -2267,6 +2286,29 @@
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C29" s="20">
+        <f t="array" ref="C29">SUMPRODUCT(D4:D19=C26,A4:A19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C30" t="str">
+        <f t="array" ref="C30">CONCATENATE(IF(OR(D4:D19=C26),"A",IF(OR(J4:J19=C26),"B",IF(OR(P4:P19=C26),"C",IF(OR(V4:V19=C26),"D","")))),IFERROR(INDEX($A4:$A19,MATCH(C26,D4:D19,0)),IFERROR(INDEX($A4:$A19,MATCH(C26,J4:J19,0)),IFERROR(INDEX($A4:$A19,MATCH(C26,P4:P19,0)),IFERROR(INDEX($A4:$A19,MATCH(C26,V4:V19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f t="array" ref="C31">IF(OR(D4:D19=C26),1,0)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2286,12 +2328,805 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="21" t="str">
+        <f t="array" ref="E3">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B3+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B3+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B3+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B3+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B3+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B3+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B3+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B3+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F3" s="21" t="str">
+        <f t="array" ref="F3">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C3+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C3+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C3+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C3+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C3+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C3+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C3+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C3+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H3" s="21" t="str">
+        <f t="array" ref="H3">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B3+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B3+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B3+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B3+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B3+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B3+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B3+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B3+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I3" s="21" t="str">
+        <f t="array" ref="I3">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C3+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C3+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C3+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C3+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C3+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C3+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C3+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C3+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>B3+2</f>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>C3+2</f>
+        <v>4</v>
+      </c>
+      <c r="E4" s="21" t="str">
+        <f t="array" ref="E4">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B4+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B4+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B4+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B4+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B4+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B4+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B4+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B4+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F4" s="21" t="str">
+        <f t="array" ref="F4">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C4+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C4+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C4+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C4+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C4+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C4+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C4+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C4+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H4" s="21" t="str">
+        <f t="array" ref="H4">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B4+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B4+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B4+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B4+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B4+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B4+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B4+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B4+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I4" s="21" t="str">
+        <f t="array" ref="I4">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C4+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C4+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C4+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C4+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C4+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C4+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C4+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C4+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f>B4+2</f>
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C26" si="0">C4+2</f>
+        <v>6</v>
+      </c>
+      <c r="E5" s="21" t="str">
+        <f t="array" ref="E5">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B5+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B5+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B5+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B5+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B5+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B5+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B5+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B5+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F5" s="21" t="str">
+        <f t="array" ref="F5">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C5+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C5+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C5+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C5+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C5+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C5+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C5+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C5+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H5" s="21" t="str">
+        <f t="array" ref="H5">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B5+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B5+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B5+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B5+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B5+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B5+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B5+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B5+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I5" s="21" t="str">
+        <f t="array" ref="I5">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C5+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C5+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C5+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C5+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C5+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C5+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C5+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C5+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" ref="B6:B26" si="1">B5+2</f>
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E6" s="21" t="str">
+        <f t="array" ref="E6">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B6+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B6+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B6+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B6+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B6+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B6+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B6+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B6+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F6" s="21" t="str">
+        <f t="array" ref="F6">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C6+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C6+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C6+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C6+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C6+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C6+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C6+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C6+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H6" s="21" t="str">
+        <f t="array" ref="H6">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B6+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B6+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B6+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B6+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B6+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B6+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B6+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B6+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I6" s="21" t="str">
+        <f t="array" ref="I6">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C6+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C6+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C6+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C6+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C6+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C6+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C6+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C6+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E7" s="21" t="str">
+        <f t="array" ref="E7">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B7+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B7+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B7+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B7+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B7+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B7+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B7+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B7+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F7" s="21" t="str">
+        <f t="array" ref="F7">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C7+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C7+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C7+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C7+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C7+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C7+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C7+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C7+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H7" s="21" t="str">
+        <f t="array" ref="H7">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B7+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B7+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B7+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B7+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B7+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B7+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B7+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B7+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I7" s="21" t="str">
+        <f t="array" ref="I7">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C7+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C7+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C7+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C7+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C7+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C7+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C7+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C7+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E8" s="21" t="str">
+        <f t="array" ref="E8">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B8+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B8+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B8+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B8+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B8+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B8+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B8+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B8+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F8" s="21" t="str">
+        <f t="array" ref="F8">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C8+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C8+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C8+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C8+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C8+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C8+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C8+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C8+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H8" s="21" t="str">
+        <f t="array" ref="H8">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B8+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B8+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B8+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B8+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B8+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B8+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B8+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B8+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I8" s="21" t="str">
+        <f t="array" ref="I8">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C8+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C8+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C8+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C8+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C8+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C8+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C8+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C8+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="21" t="str">
+        <f t="array" ref="E9">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B9+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B9+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B9+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B9+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B9+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B9+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B9+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B9+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F9" s="21" t="str">
+        <f t="array" ref="F9">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C9+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C9+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C9+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C9+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C9+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C9+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C9+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C9+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H9" s="21" t="str">
+        <f t="array" ref="H9">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B9+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B9+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B9+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B9+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B9+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B9+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B9+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B9+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B9</v>
+      </c>
+      <c r="I9" s="21" t="str">
+        <f t="array" ref="I9">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C9+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C9+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C9+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C9+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C9+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C9+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C9+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C9+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E10" s="21" t="str">
+        <f t="array" ref="E10">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B10+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B10+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B10+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B10+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B10+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B10+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B10+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B10+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F10" s="21" t="str">
+        <f t="array" ref="F10">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C10+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C10+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C10+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C10+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C10+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C10+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C10+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C10+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C13</v>
+      </c>
+      <c r="H10" s="21" t="str">
+        <f t="array" ref="H10">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B10+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B10+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B10+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B10+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B10+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B10+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B10+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B10+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B7</v>
+      </c>
+      <c r="I10" s="21" t="str">
+        <f t="array" ref="I10">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C10+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C10+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C10+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C10+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C10+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C10+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C10+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C10+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E11" s="21" t="str">
+        <f t="array" ref="E11">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B11+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B11+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B11+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B11+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B11+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B11+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B11+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B11+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C0</v>
+      </c>
+      <c r="F11" s="21" t="str">
+        <f t="array" ref="F11">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C11+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C11+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C11+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C11+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C11+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C11+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C11+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C11+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C1</v>
+      </c>
+      <c r="H11" s="21" t="str">
+        <f t="array" ref="H11">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B11+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B11+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B11+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B11+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B11+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B11+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B11+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B11+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B5</v>
+      </c>
+      <c r="I11" s="21" t="str">
+        <f t="array" ref="I11">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C11+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C11+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C11+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C11+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C11+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C11+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C11+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C11+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E12" s="21" t="str">
+        <f t="array" ref="E12">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B12+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B12+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B12+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B12+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B12+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B12+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B12+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B12+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C2</v>
+      </c>
+      <c r="F12" s="21" t="str">
+        <f t="array" ref="F12">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C12+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C12+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C12+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C12+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C12+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C12+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C12+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C12+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C3</v>
+      </c>
+      <c r="H12" s="21" t="str">
+        <f t="array" ref="H12">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B12+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B12+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B12+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B12+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B12+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B12+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B12+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B12+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D7</v>
+      </c>
+      <c r="I12" s="21" t="str">
+        <f t="array" ref="I12">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C12+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C12+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C12+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C12+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C12+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C12+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C12+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C12+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E13" s="21" t="str">
+        <f t="array" ref="E13">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B13+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B13+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B13+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B13+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B13+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B13+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B13+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B13+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F13" s="21" t="str">
+        <f t="array" ref="F13">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C13+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C13+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C13+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C13+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C13+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C13+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C13+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C13+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H13" s="21" t="str">
+        <f t="array" ref="H13">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B13+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B13+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B13+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B13+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B13+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B13+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B13+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B13+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D5</v>
+      </c>
+      <c r="I13" s="21" t="str">
+        <f t="array" ref="I13">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C13+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C13+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C13+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C13+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C13+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C13+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C13+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C13+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E14" s="21" t="str">
+        <f t="array" ref="E14">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B14+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B14+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B14+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B14+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B14+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B14+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B14+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B14+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A0</v>
+      </c>
+      <c r="F14" s="21" t="str">
+        <f t="array" ref="F14">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C14+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C14+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C14+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C14+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C14+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C14+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C14+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C14+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A1</v>
+      </c>
+      <c r="H14" s="21" t="str">
+        <f t="array" ref="H14">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B14+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B14+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B14+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B14+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B14+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B14+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B14+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B14+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D3</v>
+      </c>
+      <c r="I14" s="21" t="str">
+        <f t="array" ref="I14">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C14+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C14+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C14+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C14+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C14+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C14+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C14+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C14+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E15" s="21" t="str">
+        <f t="array" ref="E15">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B15+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B15+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B15+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B15+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B15+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B15+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B15+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B15+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A2</v>
+      </c>
+      <c r="F15" s="21" t="str">
+        <f t="array" ref="F15">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C15+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C15+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C15+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C15+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C15+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C15+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C15+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C15+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A3</v>
+      </c>
+      <c r="H15" s="21" t="str">
+        <f t="array" ref="H15">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B15+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B15+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B15+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B15+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B15+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B15+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B15+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B15+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D1</v>
+      </c>
+      <c r="I15" s="21" t="str">
+        <f t="array" ref="I15">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C15+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C15+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C15+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C15+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C15+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C15+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C15+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C15+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E16" s="21" t="str">
+        <f t="array" ref="E16">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B16+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B16+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B16+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B16+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B16+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B16+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B16+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B16+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A4</v>
+      </c>
+      <c r="F16" s="21" t="str">
+        <f t="array" ref="F16">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C16+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C16+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C16+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C16+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C16+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C16+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C16+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C16+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A5</v>
+      </c>
+      <c r="H16" s="21" t="str">
+        <f t="array" ref="H16">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B16+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B16+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B16+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B16+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B16+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B16+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B16+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B16+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C12</v>
+      </c>
+      <c r="I16" s="21" t="str">
+        <f t="array" ref="I16">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C16+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C16+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C16+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C16+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C16+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C16+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C16+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C16+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E17" s="21" t="str">
+        <f t="array" ref="E17">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B17+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B17+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B17+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B17+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B17+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B17+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B17+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B17+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A6</v>
+      </c>
+      <c r="F17" s="21" t="str">
+        <f t="array" ref="F17">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C17+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C17+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C17+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C17+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C17+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C17+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C17+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C17+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A7</v>
+      </c>
+      <c r="H17" s="21" t="str">
+        <f t="array" ref="H17">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B17+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B17+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B17+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B17+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B17+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B17+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B17+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B17+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C10</v>
+      </c>
+      <c r="I17" s="21" t="str">
+        <f t="array" ref="I17">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C17+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C17+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C17+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C17+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C17+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C17+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C17+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C17+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E18" s="21" t="str">
+        <f t="array" ref="E18">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B18+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B18+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B18+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B18+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B18+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B18+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B18+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B18+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C4</v>
+      </c>
+      <c r="F18" s="21" t="str">
+        <f t="array" ref="F18">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C18+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C18+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C18+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C18+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C18+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C18+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C18+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C18+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C5</v>
+      </c>
+      <c r="H18" s="21" t="str">
+        <f t="array" ref="H18">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B18+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B18+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B18+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B18+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B18+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B18+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B18+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B18+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A12</v>
+      </c>
+      <c r="I18" s="21" t="str">
+        <f t="array" ref="I18">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C18+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C18+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C18+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C18+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C18+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C18+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C18+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C18+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E19" s="21" t="str">
+        <f t="array" ref="E19">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B19+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B19+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B19+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B19+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B19+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B19+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B19+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B19+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B0</v>
+      </c>
+      <c r="F19" s="21" t="str">
+        <f t="array" ref="F19">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C19+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C19+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C19+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C19+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C19+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C19+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C19+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C19+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B1</v>
+      </c>
+      <c r="H19" s="21" t="str">
+        <f t="array" ref="H19">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B19+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B19+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B19+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B19+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B19+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B19+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B19+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B19+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A10</v>
+      </c>
+      <c r="I19" s="21" t="str">
+        <f t="array" ref="I19">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C19+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C19+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C19+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C19+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C19+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C19+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C19+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C19+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E20" s="21" t="str">
+        <f t="array" ref="E20">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B20+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B20+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B20+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B20+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B20+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B20+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B20+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B20+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F20" s="21" t="str">
+        <f t="array" ref="F20">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C20+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C20+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C20+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C20+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C20+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C20+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C20+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C20+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H20" s="21" t="str">
+        <f t="array" ref="H20">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B20+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B20+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B20+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B20+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B20+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B20+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B20+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B20+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>A8</v>
+      </c>
+      <c r="I20" s="21" t="str">
+        <f t="array" ref="I20">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C20+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C20+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C20+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C20+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C20+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C20+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C20+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C20+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E21" s="21" t="str">
+        <f t="array" ref="E21">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B21+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B21+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B21+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B21+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B21+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B21+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B21+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B21+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F21" s="21" t="str">
+        <f t="array" ref="F21">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C21+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C21+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C21+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C21+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C21+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C21+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C21+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C21+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H21" s="21" t="str">
+        <f t="array" ref="H21">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B21+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B21+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B21+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B21+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B21+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B21+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B21+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B21+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C8</v>
+      </c>
+      <c r="I21" s="21" t="str">
+        <f t="array" ref="I21">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C21+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C21+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C21+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C21+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C21+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C21+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C21+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C21+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E22" s="21" t="str">
+        <f t="array" ref="E22">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B22+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B22+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B22+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B22+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B22+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B22+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B22+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B22+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F22" s="21" t="str">
+        <f t="array" ref="F22">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C22+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C22+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C22+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C22+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C22+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C22+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C22+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C22+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H22" s="21" t="str">
+        <f t="array" ref="H22">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B22+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B22+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B22+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B22+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B22+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B22+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B22+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B22+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>C6</v>
+      </c>
+      <c r="I22" s="21" t="str">
+        <f t="array" ref="I22">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C22+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C22+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C22+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C22+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C22+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C22+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C22+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C22+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E23" s="21" t="str">
+        <f t="array" ref="E23">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B23+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B23+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B23+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B23+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B23+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B23+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B23+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B23+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F23" s="21" t="str">
+        <f t="array" ref="F23">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C23+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C23+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C23+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C23+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C23+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C23+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C23+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C23+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H23" s="21" t="str">
+        <f t="array" ref="H23">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B23+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B23+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B23+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B23+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B23+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B23+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B23+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B23+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D14</v>
+      </c>
+      <c r="I23" s="21" t="str">
+        <f t="array" ref="I23">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C23+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C23+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C23+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C23+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C23+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C23+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C23+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C23+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E24" s="21" t="str">
+        <f t="array" ref="E24">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B24+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B24+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B24+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B24+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B24+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B24+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B24+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B24+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F24" s="21" t="str">
+        <f t="array" ref="F24">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C24+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C24+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C24+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C24+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C24+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C24+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C24+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C24+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B10</v>
+      </c>
+      <c r="H24" s="21" t="str">
+        <f t="array" ref="H24">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B24+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B24+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B24+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B24+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B24+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B24+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B24+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B24+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D12</v>
+      </c>
+      <c r="I24" s="21" t="str">
+        <f t="array" ref="I24">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C24+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C24+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C24+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C24+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C24+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C24+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C24+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C24+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D11</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="E25" s="21" t="str">
+        <f t="array" ref="E25">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B25+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B25+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B25+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B25+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B25+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B25+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B25+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B25+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B11</v>
+      </c>
+      <c r="F25" s="21" t="str">
+        <f t="array" ref="F25">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C25+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C25+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C25+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C25+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C25+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C25+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C25+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C25+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B12</v>
+      </c>
+      <c r="H25" s="21" t="str">
+        <f t="array" ref="H25">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B25+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B25+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B25+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B25+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B25+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B25+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B25+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B25+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D10</v>
+      </c>
+      <c r="I25" s="21" t="str">
+        <f t="array" ref="I25">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C25+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C25+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C25+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C25+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C25+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C25+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C25+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C25+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E26" s="21" t="str">
+        <f t="array" ref="E26">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B26+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B26+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B26+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B26+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B26+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B26+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B26+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B26+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B13</v>
+      </c>
+      <c r="F26" s="21" t="str">
+        <f t="array" ref="F26">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C26+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C26+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C26+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C26+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C26+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C26+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C26+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C26+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B14</v>
+      </c>
+      <c r="H26" s="21" t="str">
+        <f t="array" ref="H26">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B26+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B26+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B26+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B26+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B26+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B26+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B26+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B26+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>D8</v>
+      </c>
+      <c r="I26" s="21" t="str">
+        <f t="array" ref="I26">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C26+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C26+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C26+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C26+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C26+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C26+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C26+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C26+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v>B15</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f t="shared" ref="B27:B36" si="2">B26+2</f>
+        <v>49</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27:C36" si="3">C26+2</f>
+        <v>50</v>
+      </c>
+      <c r="E27" s="21" t="str">
+        <f t="array" ref="E27">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B27+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B27+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B27+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B27+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B27+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B27+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B27+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B27+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F27" s="21" t="str">
+        <f t="array" ref="F27">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C27+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C27+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C27+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C27+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C27+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C27+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C27+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C27+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H27" s="21" t="str">
+        <f t="array" ref="H27">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B27+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B27+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B27+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B27+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B27+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B27+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B27+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B27+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I27" s="21" t="str">
+        <f t="array" ref="I27">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C27+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C27+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C27+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C27+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C27+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C27+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C27+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C27+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="E28" s="21" t="str">
+        <f t="array" ref="E28">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B28+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B28+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B28+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B28+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B28+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B28+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B28+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B28+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F28" s="21" t="str">
+        <f t="array" ref="F28">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C28+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C28+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C28+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C28+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C28+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C28+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C28+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C28+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H28" s="21" t="str">
+        <f t="array" ref="H28">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B28+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B28+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B28+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B28+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B28+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B28+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B28+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B28+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I28" s="21" t="str">
+        <f t="array" ref="I28">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C28+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C28+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C28+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C28+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C28+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C28+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C28+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C28+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="E29" s="21" t="str">
+        <f t="array" ref="E29">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B29+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B29+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B29+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B29+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B29+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B29+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B29+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B29+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F29" s="21" t="str">
+        <f t="array" ref="F29">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C29+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C29+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C29+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C29+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C29+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C29+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C29+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C29+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H29" s="21" t="str">
+        <f t="array" ref="H29">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B29+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B29+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B29+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B29+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B29+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B29+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B29+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B29+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I29" s="21" t="str">
+        <f t="array" ref="I29">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C29+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C29+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C29+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C29+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C29+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C29+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C29+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C29+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="E30" s="21" t="str">
+        <f t="array" ref="E30">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B30+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B30+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B30+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B30+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B30+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B30+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B30+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B30+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F30" s="21" t="str">
+        <f t="array" ref="F30">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C30+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C30+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C30+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C30+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C30+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C30+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C30+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C30+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H30" s="21" t="str">
+        <f t="array" ref="H30">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B30+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B30+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B30+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B30+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B30+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B30+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B30+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B30+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I30" s="21" t="str">
+        <f t="array" ref="I30">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C30+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C30+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C30+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C30+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C30+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C30+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C30+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C30+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="E31" s="21" t="str">
+        <f t="array" ref="E31">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B31+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B31+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B31+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B31+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B31+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B31+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B31+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B31+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F31" s="21" t="str">
+        <f t="array" ref="F31">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C31+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C31+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C31+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C31+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C31+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C31+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C31+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C31+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H31" s="21" t="str">
+        <f t="array" ref="H31">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B31+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B31+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B31+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B31+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B31+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B31+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B31+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B31+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I31" s="21" t="str">
+        <f t="array" ref="I31">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C31+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C31+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C31+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C31+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C31+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C31+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C31+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C31+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="E32" s="21" t="str">
+        <f t="array" ref="E32">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B32+E$2),"A",IF(OR(Лист1!$J$4:$J$19=$B32+E$2),"B",IF(OR(Лист1!$P$4:$P$19=$B32+E$2),"C",IF(OR(Лист1!$V$4:$V$19=$B32+E$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B32+E$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B32+E$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B32+E$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B32+E$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="F32" s="21" t="str">
+        <f t="array" ref="F32">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C32+F$2),"A",IF(OR(Лист1!$J$4:$J$19=$C32+F$2),"B",IF(OR(Лист1!$P$4:$P$19=$C32+F$2),"C",IF(OR(Лист1!$V$4:$V$19=$C32+F$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C32+F$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C32+F$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C32+F$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C32+F$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="H32" s="21" t="str">
+        <f t="array" ref="H32">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$B32+H$2),"A",IF(OR(Лист1!$J$4:$J$19=$B32+H$2),"B",IF(OR(Лист1!$P$4:$P$19=$B32+H$2),"C",IF(OR(Лист1!$V$4:$V$19=$B32+H$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B32+H$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B32+H$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B32+H$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($B32+H$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+      <c r="I32" s="21" t="str">
+        <f t="array" ref="I32">CONCATENATE(IF(OR(Лист1!$D$4:$D$19=$C32+I$2),"A",IF(OR(Лист1!$J$4:$J$19=$C32+I$2),"B",IF(OR(Лист1!$P$4:$P$19=$C32+I$2),"C",IF(OR(Лист1!$V$4:$V$19=$C32+I$2),"D","")))),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C32+I$2,Лист1!$D$4:$D$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C32+I$2,Лист1!$J$4:$J$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C32+I$2,Лист1!$P$4:$P$19,0)),IFERROR(INDEX(Лист1!$A$4:$A$19,MATCH($C32+I$2,Лист1!$V$4:$V$19,0)),"")))))</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>